<commit_message>
add xlsx and csv
</commit_message>
<xml_diff>
--- a/inst/extdata/df_aae.xlsx
+++ b/inst/extdata/df_aae.xlsx
@@ -5514,7 +5514,7 @@
         <v>3530707.81556976</v>
       </c>
       <c r="L31" t="n">
-        <v>1142368.9539026</v>
+        <v>1142368.95390259</v>
       </c>
       <c r="M31" s="1" t="n">
         <v>45062.71875</v>
@@ -5644,7 +5644,7 @@
         <v>3586289.53095729</v>
       </c>
       <c r="L33" t="n">
-        <v>1188500.5846741</v>
+        <v>1188500.58467411</v>
       </c>
       <c r="M33" s="1" t="n">
         <v>45071.3475694444</v>
@@ -11996,7 +11996,7 @@
         <v>-15.7957795858383</v>
       </c>
       <c r="F131" t="n">
-        <v>35.002965333173</v>
+        <v>35.0029653331731</v>
       </c>
       <c r="G131" t="n">
         <v>127897</v>
@@ -14224,7 +14224,7 @@
         <v>5085352.89257436</v>
       </c>
       <c r="L165" t="n">
-        <v>1147039.7231336</v>
+        <v>1147039.72313359</v>
       </c>
       <c r="M165" s="1" t="n">
         <v>45071.7698032407</v>
@@ -15849,7 +15849,7 @@
         <v>15392658.5546533</v>
       </c>
       <c r="L190" t="n">
-        <v>7508207.0465248</v>
+        <v>7508207.04652481</v>
       </c>
       <c r="M190" s="1" t="n">
         <v>45072.4204976852</v>
@@ -18106,7 +18106,7 @@
         <v>-15.7957779765129</v>
       </c>
       <c r="F225" t="n">
-        <v>35.002962499857</v>
+        <v>35.0029624998569</v>
       </c>
       <c r="G225" t="n">
         <v>3939</v>
@@ -18821,7 +18821,7 @@
         <v>-15.7957534790039</v>
       </c>
       <c r="F236" t="n">
-        <v>35.002962499857</v>
+        <v>35.0029624998569</v>
       </c>
       <c r="G236" t="n">
         <v>143170</v>
@@ -21746,7 +21746,7 @@
         <v>-15.7957223057747</v>
       </c>
       <c r="F281" t="n">
-        <v>35.002942999592</v>
+        <v>35.0029429995921</v>
       </c>
       <c r="G281" t="n">
         <v>144384</v>
@@ -30279,7 +30279,7 @@
         <v>19876411.6241192</v>
       </c>
       <c r="L412" t="n">
-        <v>7909893.2003908</v>
+        <v>7909893.20039081</v>
       </c>
       <c r="M412" s="1" t="n">
         <v>45072.7347337963</v>
@@ -30976,7 +30976,7 @@
         <v>-15.7957871556282</v>
       </c>
       <c r="F423" t="n">
-        <v>35.002962499857</v>
+        <v>35.0029624998569</v>
       </c>
       <c r="G423" t="n">
         <v>45988</v>
@@ -31496,7 +31496,7 @@
         <v>-15.7958036661148</v>
       </c>
       <c r="F431" t="n">
-        <v>35.002962499857</v>
+        <v>35.0029624998569</v>
       </c>
       <c r="G431" t="n">
         <v>287709</v>
@@ -31514,7 +31514,7 @@
         <v>4134287.98483218</v>
       </c>
       <c r="L431" t="n">
-        <v>1806240.9539354</v>
+        <v>1806240.95393539</v>
       </c>
       <c r="M431" s="1" t="n">
         <v>45072.7416782407</v>
@@ -36628,7 +36628,7 @@
         <v>444</v>
       </c>
       <c r="E510" t="n">
-        <v>-15.79571133852</v>
+        <v>-15.7957113385201</v>
       </c>
       <c r="F510" t="n">
         <v>35.0029641664587</v>
@@ -39816,7 +39816,7 @@
         <v>-15.7957681417465</v>
       </c>
       <c r="F559" t="n">
-        <v>35.002965333173</v>
+        <v>35.0029653331731</v>
       </c>
       <c r="G559" t="n">
         <v>33974</v>
@@ -40661,7 +40661,7 @@
         <v>-15.7957681417465</v>
       </c>
       <c r="F572" t="n">
-        <v>35.002965333173</v>
+        <v>35.0029653331731</v>
       </c>
       <c r="G572" t="n">
         <v>218805</v>
@@ -52964,7 +52964,7 @@
         <v>10785258.5390271</v>
       </c>
       <c r="L761" t="n">
-        <v>2614642.1232061</v>
+        <v>2614642.12320611</v>
       </c>
       <c r="M761" s="1" t="n">
         <v>45075.5006944444</v>
@@ -53726,7 +53726,7 @@
         <v>-15.7989467978477</v>
       </c>
       <c r="F773" t="n">
-        <v>35.02661816217</v>
+        <v>35.0266181621701</v>
       </c>
       <c r="G773" t="n">
         <v>-2165</v>
@@ -54568,7 +54568,7 @@
         <v>683</v>
       </c>
       <c r="E786" t="n">
-        <v>-15.814984202385</v>
+        <v>-15.8149842023849</v>
       </c>
       <c r="F786" t="n">
         <v>35.0610374882817</v>
@@ -60031,7 +60031,7 @@
         <v>-15.8137314915657</v>
       </c>
       <c r="F870" t="n">
-        <v>35.060294996947</v>
+        <v>35.0602949969471</v>
       </c>
       <c r="G870" t="n">
         <v>5540</v>
@@ -66008,7 +66008,7 @@
         <v>829</v>
       </c>
       <c r="E962" t="n">
-        <v>-15.817345738411</v>
+        <v>-15.8173457384109</v>
       </c>
       <c r="F962" t="n">
         <v>34.9969847202301</v>
@@ -75436,7 +75436,7 @@
         <v>-15.7871858477592</v>
       </c>
       <c r="F1107" t="n">
-        <v>35.034411828965</v>
+        <v>35.0344118289649</v>
       </c>
       <c r="G1107" t="n">
         <v>20870</v>
@@ -76169,7 +76169,7 @@
         <v>3243190.89247776</v>
       </c>
       <c r="L1118" t="n">
-        <v>1456914.1231489</v>
+        <v>1456914.12314891</v>
       </c>
       <c r="M1118" s="1" t="n">
         <v>45077.4225810185</v>
@@ -79011,7 +79011,7 @@
         <v>-15.8028050065041</v>
       </c>
       <c r="F1162" t="n">
-        <v>35.018657328561</v>
+        <v>35.0186573285609</v>
       </c>
       <c r="G1162" t="n">
         <v>-229</v>
@@ -80051,7 +80051,7 @@
         <v>-15.8028460741043</v>
       </c>
       <c r="F1178" t="n">
-        <v>35.018711162731</v>
+        <v>35.0187111627311</v>
       </c>
       <c r="G1178" t="n">
         <v>-275</v>

</xml_diff>